<commit_message>
Complete: question files are completed
</commit_message>
<xml_diff>
--- a/assets/questions/questions.xlsx
+++ b/assets/questions/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthor\Documents\Fullstack\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3531A69-7C06-4184-81D3-CCA7705375AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84804641-911A-4B5B-A5B0-4795C1C00BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86148A14-0F71-4793-B760-0F84D180BEDC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="450">
   <si>
     <t>Question</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Derek K Dick is better known as?</t>
   </si>
   <si>
-    <t>Sisters are doin it for themselves was a hit for?</t>
-  </si>
-  <si>
     <t>Who did a duet with Dancing in the streets together with David Bowie?</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>Dont you forget about me</t>
   </si>
   <si>
-    <t>Shakin Stevens</t>
-  </si>
-  <si>
     <t>Annie Lennox</t>
   </si>
   <si>
@@ -395,9 +389,6 @@
     <t>Radio Ga-Ga</t>
   </si>
   <si>
-    <t>Im going slightly mad</t>
-  </si>
-  <si>
     <t>We will rock you</t>
   </si>
   <si>
@@ -677,9 +668,6 @@
     <t>Van Halen</t>
   </si>
   <si>
-    <t>Guns n roses</t>
-  </si>
-  <si>
     <t>Mark Chapel</t>
   </si>
   <si>
@@ -798,13 +786,637 @@
   </si>
   <si>
     <t>Eternal</t>
+  </si>
+  <si>
+    <t>The german band Kraftwerk was founded in which City?</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Düsseldorf</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>What is the name of The Beatles’ first album?</t>
+  </si>
+  <si>
+    <t>Which Canadian artist released 'Man! I Feel Like A Woman!’ in 1999?</t>
+  </si>
+  <si>
+    <t>Please Please Me</t>
+  </si>
+  <si>
+    <t>Billy Ray Cyrus</t>
+  </si>
+  <si>
+    <t>Shania Twain</t>
+  </si>
+  <si>
+    <t>Bryan Adams</t>
+  </si>
+  <si>
+    <t>Celine Dion</t>
+  </si>
+  <si>
+    <t>Alanis Morissette</t>
+  </si>
+  <si>
+    <t>William Cyrus</t>
+  </si>
+  <si>
+    <t>Ron Cyrus</t>
+  </si>
+  <si>
+    <t>Gordon Cyrus</t>
+  </si>
+  <si>
+    <t>Abbey Road</t>
+  </si>
+  <si>
+    <t>Help!</t>
+  </si>
+  <si>
+    <t>Revolver</t>
+  </si>
+  <si>
+    <t>Sisters are doin' it for themselves was a hit for?</t>
+  </si>
+  <si>
+    <t>I'm going slightly mad</t>
+  </si>
+  <si>
+    <t>Guns n' roses</t>
+  </si>
+  <si>
+    <t>What is the name of Miley Cyrus father?</t>
+  </si>
+  <si>
+    <t>In which decade did Elvis have his first UK No. 1?</t>
+  </si>
+  <si>
+    <t>Who was the first to leave Take That?</t>
+  </si>
+  <si>
+    <t>Which group wrote most of the songs for the movie Saturday Night Fever?</t>
+  </si>
+  <si>
+    <t>1950s</t>
+  </si>
+  <si>
+    <t>1960s</t>
+  </si>
+  <si>
+    <t>1970s</t>
+  </si>
+  <si>
+    <t>1940s</t>
+  </si>
+  <si>
+    <t>Robbie Williams</t>
+  </si>
+  <si>
+    <t>Jason Orange</t>
+  </si>
+  <si>
+    <t>Gary Barlow</t>
+  </si>
+  <si>
+    <t>Boney M</t>
+  </si>
+  <si>
+    <t>Chic</t>
+  </si>
+  <si>
+    <t>Village People</t>
+  </si>
+  <si>
+    <t>Shakin' Stevens</t>
+  </si>
+  <si>
+    <t>What is ABBA:s breakthru song?</t>
+  </si>
+  <si>
+    <t>Dancing Queen</t>
+  </si>
+  <si>
+    <t>When I kissed the teacher</t>
+  </si>
+  <si>
+    <t>Waterloo</t>
+  </si>
+  <si>
+    <t>Money, Money, Money</t>
+  </si>
+  <si>
+    <t>Phil Collins plays what instrument?</t>
+  </si>
+  <si>
+    <t>Guitar</t>
+  </si>
+  <si>
+    <t>Bass</t>
+  </si>
+  <si>
+    <t>Drum</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>The industrial band Nine inch Nails released the debut album in 1989. What is it called?</t>
+  </si>
+  <si>
+    <t>Pretty Hate Machine</t>
+  </si>
+  <si>
+    <t>The Fragile</t>
+  </si>
+  <si>
+    <t>The Downward Spiral</t>
+  </si>
+  <si>
+    <t>With Teeth</t>
+  </si>
+  <si>
+    <t>"Crazy in Love" was the first solo No. 1 for which singer?</t>
+  </si>
+  <si>
+    <t>Beyonce</t>
+  </si>
+  <si>
+    <t>Miley Cirus</t>
+  </si>
+  <si>
+    <t>Adele</t>
+  </si>
+  <si>
+    <t>According to the name of a hit by Paul Hardcastle, how old was the average american soldier in the Vietnam war?</t>
+  </si>
+  <si>
+    <t>Which Brittish band gave us "Lessons in love"?</t>
+  </si>
+  <si>
+    <t>Level 42</t>
+  </si>
+  <si>
+    <t>Wham!</t>
+  </si>
+  <si>
+    <t>Tears for Fears</t>
+  </si>
+  <si>
+    <t>Who was the first singer of Iron Maiden?</t>
+  </si>
+  <si>
+    <t>Paul Day</t>
+  </si>
+  <si>
+    <t>Bruce Dickinson</t>
+  </si>
+  <si>
+    <t>Paul Di'Anno</t>
+  </si>
+  <si>
+    <t>Blaze Bayley</t>
+  </si>
+  <si>
+    <t>David Bowies real surname is?</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Which Scottish band released Take Me Out in 2004?</t>
+  </si>
+  <si>
+    <t>Franz Ferdinand</t>
+  </si>
+  <si>
+    <t>Primal Scream</t>
+  </si>
+  <si>
+    <t>Big Country</t>
+  </si>
+  <si>
+    <t>Belle and Sebastian</t>
+  </si>
+  <si>
+    <t>What was Lady Gaga's first No. 1 hit?</t>
+  </si>
+  <si>
+    <t>Just Dance</t>
+  </si>
+  <si>
+    <t>Bad Romance</t>
+  </si>
+  <si>
+    <t>Poker Face</t>
+  </si>
+  <si>
+    <t>Government Hooker</t>
+  </si>
+  <si>
+    <t>Who was the first person to win Britain's Got Talent?</t>
+  </si>
+  <si>
+    <t>Paul Potts</t>
+  </si>
+  <si>
+    <t>What song by PSY was the first YouTube video to be viewed 1 billion times?</t>
+  </si>
+  <si>
+    <t>Gangnam Style</t>
+  </si>
+  <si>
+    <t>What is the stage name of Anna Mae Bullock?</t>
+  </si>
+  <si>
+    <t>Which 1980's band are responsible for the hit 'Sweet Dreams (Are Made of This)'?</t>
+  </si>
+  <si>
+    <t>Eurythmics</t>
+  </si>
+  <si>
+    <t>Name the 1994 debut studio album by Oasis?</t>
+  </si>
+  <si>
+    <t>Definitely Maybe</t>
+  </si>
+  <si>
+    <t>Name the 1993 debut studio album by Suede?</t>
+  </si>
+  <si>
+    <t>Suede</t>
+  </si>
+  <si>
+    <t>Dog Man Star</t>
+  </si>
+  <si>
+    <t>Coming up</t>
+  </si>
+  <si>
+    <t>Head Music</t>
+  </si>
+  <si>
+    <t>Heavy metal band "King Diamond" is from what country?</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Susan Boyle</t>
+  </si>
+  <si>
+    <t>Jai McDowall</t>
+  </si>
+  <si>
+    <t>Calum Scott</t>
+  </si>
+  <si>
+    <t>Gentleman</t>
+  </si>
+  <si>
+    <t>Hangover</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Cher</t>
+  </si>
+  <si>
+    <t>Anastacia</t>
+  </si>
+  <si>
+    <t>The Human League</t>
+  </si>
+  <si>
+    <t>Alphaville</t>
+  </si>
+  <si>
+    <t>New Order</t>
+  </si>
+  <si>
+    <t>(What's the Story) Morning Glory?</t>
+  </si>
+  <si>
+    <t>Be Here Now</t>
+  </si>
+  <si>
+    <t>Standing on the shoulders of giants</t>
+  </si>
+  <si>
+    <t>Who wrote the song 'Let's Get It On'?</t>
+  </si>
+  <si>
+    <t>Marvin Gaye</t>
+  </si>
+  <si>
+    <t>'You Spin Me Round (Like a Record)' is a song by which British band?</t>
+  </si>
+  <si>
+    <t>Dead or alive</t>
+  </si>
+  <si>
+    <t>How old was Mozart when he wrote his first piece?</t>
+  </si>
+  <si>
+    <t>Who is the only member of ZZ Top that doesn't have a beard?</t>
+  </si>
+  <si>
+    <t>Frank Beard</t>
+  </si>
+  <si>
+    <t>T Rex was led by which singer?</t>
+  </si>
+  <si>
+    <t>Marc Bolan</t>
+  </si>
+  <si>
+    <t>Which Jamaican artist released a song in 1974 that begins with the lyrics, 'Everybody was Kung Fu fighting'?</t>
+  </si>
+  <si>
+    <t>Carl Douglas</t>
+  </si>
+  <si>
+    <t>Which Pink Floyd album featured the song 'Comfortably Numb'?</t>
+  </si>
+  <si>
+    <t>The Wall</t>
+  </si>
+  <si>
+    <t>Which famous music group were formerly known as the New Yardbirds?</t>
+  </si>
+  <si>
+    <t>Led Zeppelin</t>
+  </si>
+  <si>
+    <t>Which British band had the hit 'Fools Gold'?</t>
+  </si>
+  <si>
+    <t>The Stone Roses</t>
+  </si>
+  <si>
+    <t>Which song gave Madonna her first UK number one?</t>
+  </si>
+  <si>
+    <t>Into the Groove</t>
+  </si>
+  <si>
+    <t>La Isla Bonita</t>
+  </si>
+  <si>
+    <t>Material Girl</t>
+  </si>
+  <si>
+    <t>Ray Charles</t>
+  </si>
+  <si>
+    <t>Stevie Wonder</t>
+  </si>
+  <si>
+    <t>Barry White</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Dire Straits</t>
+  </si>
+  <si>
+    <t>Billy Gibbons</t>
+  </si>
+  <si>
+    <t>Dusty Hill</t>
+  </si>
+  <si>
+    <t>Billy Ethridge</t>
+  </si>
+  <si>
+    <t>Steve Currie</t>
+  </si>
+  <si>
+    <t>Herbie Flowers</t>
+  </si>
+  <si>
+    <t>Tony Newman</t>
+  </si>
+  <si>
+    <t>Shaggy</t>
+  </si>
+  <si>
+    <t>Buju Banton</t>
+  </si>
+  <si>
+    <t>Sean Paul</t>
+  </si>
+  <si>
+    <t>The Dark Side of the Moon</t>
+  </si>
+  <si>
+    <t>Wish you were here</t>
+  </si>
+  <si>
+    <t>The Division Bell</t>
+  </si>
+  <si>
+    <t>Radiohead</t>
+  </si>
+  <si>
+    <t>Pearl Jam</t>
+  </si>
+  <si>
+    <t>Blur</t>
+  </si>
+  <si>
+    <t>Def Leppard</t>
+  </si>
+  <si>
+    <t>Saxon</t>
+  </si>
+  <si>
+    <t>Black Sabbath</t>
+  </si>
+  <si>
+    <t>Which band is NOT considered one of the Big Four of thrash metal?</t>
+  </si>
+  <si>
+    <t>Metallica</t>
+  </si>
+  <si>
+    <t>Slayer</t>
+  </si>
+  <si>
+    <t>Megadeth</t>
+  </si>
+  <si>
+    <t>Iron Maiden</t>
+  </si>
+  <si>
+    <t>Before Midge Ure was the singer of Ultravox, what other band was he a member of?</t>
+  </si>
+  <si>
+    <t>Visage</t>
+  </si>
+  <si>
+    <t>Yaz</t>
+  </si>
+  <si>
+    <t>Spandau Ballet</t>
+  </si>
+  <si>
+    <t>Soft Cell</t>
+  </si>
+  <si>
+    <t>The founding members of Heaven 17 left what band due to conflicts prior to starting Heaven 17?</t>
+  </si>
+  <si>
+    <t>Human League</t>
+  </si>
+  <si>
+    <t>O.M.D.</t>
+  </si>
+  <si>
+    <t>Men Without Hats</t>
+  </si>
+  <si>
+    <t>Which band is NOT from Finland?</t>
+  </si>
+  <si>
+    <t>Nightwish</t>
+  </si>
+  <si>
+    <t>Apocalyptica</t>
+  </si>
+  <si>
+    <t>Lordi</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Which famous rapper married reality TV star Kim Kardashian in 2014?</t>
+  </si>
+  <si>
+    <t>Kanye West</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>50 Cent</t>
+  </si>
+  <si>
+    <t>In 1994, the Elton John song 'Can You Feel the Love Tonight' was released. Which Disney film from the same year featured this tune?</t>
+  </si>
+  <si>
+    <t>The Lion King</t>
+  </si>
+  <si>
+    <t>Aladdin</t>
+  </si>
+  <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>A bugs life</t>
+  </si>
+  <si>
+    <t>What song by Katrina &amp; The Waves won the 1997 Eurovision Song Contest for the UK?</t>
+  </si>
+  <si>
+    <t>Love shine a light</t>
+  </si>
+  <si>
+    <t>Walking on sunshine</t>
+  </si>
+  <si>
+    <t>Sun Street</t>
+  </si>
+  <si>
+    <t>Going down to Liverpool</t>
+  </si>
+  <si>
+    <t>Who sang the song from the Titanic movie, 'My Heart Will Go On'?</t>
+  </si>
+  <si>
+    <t>"Bobby Brown" is from what Frank Zappa album?</t>
+  </si>
+  <si>
+    <t>Sheik Yerbouti</t>
+  </si>
+  <si>
+    <t>Hot Rats</t>
+  </si>
+  <si>
+    <t>The Grand Wazoo</t>
+  </si>
+  <si>
+    <t>Apostrophe</t>
+  </si>
+  <si>
+    <r>
+      <t>In 1984, Prince released his sixth studio album, entitled 'Purple Rain'</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF141414"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF141414"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t> What was the album’s lead single?</t>
+    </r>
+  </si>
+  <si>
+    <t>When doves cry</t>
+  </si>
+  <si>
+    <t>Purple rain</t>
+  </si>
+  <si>
+    <t>Let's go crazy</t>
+  </si>
+  <si>
+    <t>Baby I'm a star</t>
+  </si>
+  <si>
+    <t>The album 'Parklife' by Blur was first released in which year?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +1425,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF141414"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF141414"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color rgb="FF141414"/>
       <name val="Open Sans"/>
@@ -827,7 +1467,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -835,13 +1475,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A208CD-2593-486C-A23F-D938E8A0C20A}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F56"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1914,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1274,7 +1934,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -1417,16 +2077,16 @@
         <v>59</v>
       </c>
       <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
       </c>
       <c r="F13" t="s">
         <v>2</v>
@@ -1434,19 +2094,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
       <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>67</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
       </c>
       <c r="F14" t="s">
         <v>1</v>
@@ -1454,19 +2114,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
         <v>70</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>71</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>72</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>74</v>
       </c>
       <c r="F15" t="s">
         <v>2</v>
@@ -1474,7 +2134,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16">
         <v>1984</v>
@@ -1494,19 +2154,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -1514,19 +2174,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" t="s">
         <v>112</v>
-      </c>
-      <c r="C18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" t="s">
-        <v>114</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1534,16 +2194,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -1554,19 +2214,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>268</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -1574,19 +2234,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F21" t="s">
         <v>1</v>
@@ -1594,19 +2254,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F22" t="s">
         <v>1</v>
@@ -1614,19 +2274,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F23" t="s">
         <v>3</v>
@@ -1634,19 +2294,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
         <v>1</v>
@@ -1654,19 +2314,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
         <v>1</v>
@@ -1674,19 +2334,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
         <v>2</v>
@@ -1694,19 +2354,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
@@ -1714,19 +2374,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F28" t="s">
         <v>1</v>
@@ -1734,19 +2394,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F29" t="s">
         <v>1</v>
@@ -1754,7 +2414,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30">
         <v>19</v>
@@ -1774,19 +2434,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F31" t="s">
         <v>1</v>
@@ -1794,19 +2454,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F32" t="s">
         <v>3</v>
@@ -1814,19 +2474,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C33" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
         <v>2</v>
@@ -1834,19 +2494,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" t="s">
-        <v>109</v>
+        <v>153</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F34" t="s">
         <v>2</v>
@@ -1854,19 +2514,19 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -1874,59 +2534,59 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E36" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" t="s">
+        <v>194</v>
+      </c>
+      <c r="E38" t="s">
         <v>195</v>
-      </c>
-      <c r="C38" t="s">
-        <v>196</v>
-      </c>
-      <c r="D38" t="s">
-        <v>197</v>
-      </c>
-      <c r="E38" t="s">
-        <v>198</v>
       </c>
       <c r="F38" t="s">
         <v>2</v>
@@ -1934,7 +2594,7 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B39">
         <v>1994</v>
@@ -1954,19 +2614,19 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40" t="s">
         <v>199</v>
-      </c>
-      <c r="C40" t="s">
-        <v>200</v>
-      </c>
-      <c r="D40" t="s">
-        <v>201</v>
-      </c>
-      <c r="E40" t="s">
-        <v>202</v>
       </c>
       <c r="F40" t="s">
         <v>1</v>
@@ -1974,19 +2634,19 @@
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
@@ -1994,7 +2654,7 @@
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B42">
         <v>1982</v>
@@ -2014,13 +2674,13 @@
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C43" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -2034,19 +2694,19 @@
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E44" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F44" t="s">
         <v>1</v>
@@ -2054,19 +2714,19 @@
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D45" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E45" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="F45" t="s">
         <v>2</v>
@@ -2074,19 +2734,19 @@
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B46" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D46" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E46" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F46" t="s">
         <v>2</v>
@@ -2094,16 +2754,16 @@
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D47" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E47" t="s">
         <v>27</v>
@@ -2114,19 +2774,19 @@
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E48" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F48" t="s">
         <v>3</v>
@@ -2134,19 +2794,19 @@
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C49" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E49" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F49" t="s">
         <v>4</v>
@@ -2154,19 +2814,19 @@
     </row>
     <row r="50" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C50" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D50" t="s">
         <v>31</v>
       </c>
       <c r="E50" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F50" t="s">
         <v>2</v>
@@ -2174,19 +2834,19 @@
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B51" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C51" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D51" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E51" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F51" t="s">
         <v>4</v>
@@ -2194,7 +2854,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B52">
         <v>2020</v>
@@ -2214,19 +2874,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D53" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E53" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F53" t="s">
         <v>1</v>
@@ -2234,19 +2894,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C54" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D54" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E54" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F54" t="s">
         <v>1</v>
@@ -2254,19 +2914,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B55" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D55" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E55" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F55" t="s">
         <v>4</v>
@@ -2274,22 +2934,922 @@
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B56" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C56" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E56" t="s">
         <v>248</v>
-      </c>
-      <c r="E56" t="s">
-        <v>252</v>
       </c>
       <c r="F56" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>250</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B68">
+        <v>20</v>
+      </c>
+      <c r="C68">
+        <v>21</v>
+      </c>
+      <c r="D68">
+        <v>19</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B69" t="s">
+        <v>306</v>
+      </c>
+      <c r="C69" t="s">
+        <v>307</v>
+      </c>
+      <c r="D69" t="s">
+        <v>308</v>
+      </c>
+      <c r="E69" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" t="s">
+        <v>310</v>
+      </c>
+      <c r="C70" t="s">
+        <v>311</v>
+      </c>
+      <c r="D70" t="s">
+        <v>312</v>
+      </c>
+      <c r="E70" t="s">
+        <v>313</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B71" t="s">
+        <v>315</v>
+      </c>
+      <c r="C71" t="s">
+        <v>317</v>
+      </c>
+      <c r="D71" t="s">
+        <v>316</v>
+      </c>
+      <c r="E71" t="s">
+        <v>318</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B72" t="s">
+        <v>321</v>
+      </c>
+      <c r="C72" t="s">
+        <v>320</v>
+      </c>
+      <c r="D72" t="s">
+        <v>322</v>
+      </c>
+      <c r="E72" t="s">
+        <v>323</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B73" t="s">
+        <v>326</v>
+      </c>
+      <c r="C73" t="s">
+        <v>327</v>
+      </c>
+      <c r="D73" t="s">
+        <v>325</v>
+      </c>
+      <c r="E73" t="s">
+        <v>328</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B74" t="s">
+        <v>347</v>
+      </c>
+      <c r="C74" t="s">
+        <v>330</v>
+      </c>
+      <c r="D74" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" t="s">
+        <v>349</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75" t="s">
+        <v>350</v>
+      </c>
+      <c r="C75" t="s">
+        <v>351</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E75" t="s">
+        <v>352</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>214</v>
+      </c>
+      <c r="D76" t="s">
+        <v>353</v>
+      </c>
+      <c r="E76" t="s">
+        <v>354</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B77" t="s">
+        <v>355</v>
+      </c>
+      <c r="C77" t="s">
+        <v>335</v>
+      </c>
+      <c r="D77" t="s">
+        <v>356</v>
+      </c>
+      <c r="E77" t="s">
+        <v>357</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D78" t="s">
+        <v>359</v>
+      </c>
+      <c r="E78" t="s">
+        <v>360</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B79" t="s">
+        <v>339</v>
+      </c>
+      <c r="C79" t="s">
+        <v>340</v>
+      </c>
+      <c r="D79" t="s">
+        <v>341</v>
+      </c>
+      <c r="E79" t="s">
+        <v>342</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B80" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" t="s">
+        <v>344</v>
+      </c>
+      <c r="D80" t="s">
+        <v>345</v>
+      </c>
+      <c r="E80" t="s">
+        <v>346</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B81" t="s">
+        <v>382</v>
+      </c>
+      <c r="C81" t="s">
+        <v>362</v>
+      </c>
+      <c r="D81" t="s">
+        <v>383</v>
+      </c>
+      <c r="E81" t="s">
+        <v>384</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" t="s">
+        <v>385</v>
+      </c>
+      <c r="D82" t="s">
+        <v>364</v>
+      </c>
+      <c r="E82" t="s">
+        <v>386</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83">
+        <v>8</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
+      </c>
+      <c r="E83">
+        <v>18</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B84" t="s">
+        <v>367</v>
+      </c>
+      <c r="C84" t="s">
+        <v>387</v>
+      </c>
+      <c r="D84" t="s">
+        <v>388</v>
+      </c>
+      <c r="E84" t="s">
+        <v>389</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B85" t="s">
+        <v>390</v>
+      </c>
+      <c r="C85" t="s">
+        <v>391</v>
+      </c>
+      <c r="D85" t="s">
+        <v>369</v>
+      </c>
+      <c r="E85" t="s">
+        <v>392</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B86" t="s">
+        <v>371</v>
+      </c>
+      <c r="C86" t="s">
+        <v>393</v>
+      </c>
+      <c r="D86" t="s">
+        <v>394</v>
+      </c>
+      <c r="E86" t="s">
+        <v>395</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B87" t="s">
+        <v>396</v>
+      </c>
+      <c r="C87" t="s">
+        <v>373</v>
+      </c>
+      <c r="D87" t="s">
+        <v>397</v>
+      </c>
+      <c r="E87" t="s">
+        <v>398</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B88" t="s">
+        <v>375</v>
+      </c>
+      <c r="C88" t="s">
+        <v>399</v>
+      </c>
+      <c r="D88" t="s">
+        <v>400</v>
+      </c>
+      <c r="E88" t="s">
+        <v>401</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B89" t="s">
+        <v>402</v>
+      </c>
+      <c r="C89" t="s">
+        <v>403</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E89" t="s">
+        <v>404</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B90" t="s">
+        <v>379</v>
+      </c>
+      <c r="C90" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" t="s">
+        <v>380</v>
+      </c>
+      <c r="E90" t="s">
+        <v>381</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C91" t="s">
+        <v>407</v>
+      </c>
+      <c r="D91" t="s">
+        <v>408</v>
+      </c>
+      <c r="E91" t="s">
+        <v>409</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B92" t="s">
+        <v>411</v>
+      </c>
+      <c r="C92" t="s">
+        <v>412</v>
+      </c>
+      <c r="D92" t="s">
+        <v>413</v>
+      </c>
+      <c r="E92" t="s">
+        <v>414</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B93" t="s">
+        <v>416</v>
+      </c>
+      <c r="C93" t="s">
+        <v>417</v>
+      </c>
+      <c r="D93" t="s">
+        <v>306</v>
+      </c>
+      <c r="E93" t="s">
+        <v>418</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B94" t="s">
+        <v>420</v>
+      </c>
+      <c r="C94" t="s">
+        <v>421</v>
+      </c>
+      <c r="D94" t="s">
+        <v>422</v>
+      </c>
+      <c r="E94" t="s">
+        <v>423</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B95" t="s">
+        <v>426</v>
+      </c>
+      <c r="C95" t="s">
+        <v>425</v>
+      </c>
+      <c r="D95" t="s">
+        <v>201</v>
+      </c>
+      <c r="E95" t="s">
+        <v>427</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B96" t="s">
+        <v>429</v>
+      </c>
+      <c r="C96" t="s">
+        <v>430</v>
+      </c>
+      <c r="D96" t="s">
+        <v>431</v>
+      </c>
+      <c r="E96" t="s">
+        <v>432</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B97" t="s">
+        <v>435</v>
+      </c>
+      <c r="C97" t="s">
+        <v>434</v>
+      </c>
+      <c r="D97" t="s">
+        <v>436</v>
+      </c>
+      <c r="E97" t="s">
+        <v>437</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B98" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" t="s">
+        <v>259</v>
+      </c>
+      <c r="E98" t="s">
+        <v>214</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B99" t="s">
+        <v>441</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D99" t="s">
+        <v>442</v>
+      </c>
+      <c r="E99" t="s">
+        <v>443</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B100" t="s">
+        <v>446</v>
+      </c>
+      <c r="C100" t="s">
+        <v>445</v>
+      </c>
+      <c r="D100" t="s">
+        <v>447</v>
+      </c>
+      <c r="E100" t="s">
+        <v>448</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B101">
+        <v>1992</v>
+      </c>
+      <c r="C101">
+        <v>1993</v>
+      </c>
+      <c r="D101">
+        <v>1995</v>
+      </c>
+      <c r="E101">
+        <v>1994</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>